<commit_message>
fix: RDCC-2517 : added fix for avoiding chile deletion if update record fails in UP
</commit_message>
<xml_diff>
--- a/src/integrationTest/resources/Staff Data Upload Update.xlsx
+++ b/src/integrationTest/resources/Staff Data Upload Update.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10314"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/350950/HMCTS/rd-caseworker-ref-api/src/integrationTest/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/429962/hmcts/rd-caseworker-ref-api/src/integrationTest/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FBCD988-8E9D-D848-9BDA-26293DB06A20}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9395FCD4-95EE-A84D-A849-4D658012C21B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14500" activeTab="2" xr2:uid="{C3779BBE-D7A5-4756-9223-DEADF9C5B8AB}"/>
+    <workbookView xWindow="800" yWindow="5140" windowWidth="25600" windowHeight="14500" activeTab="2" xr2:uid="{C3779BBE-D7A5-4756-9223-DEADF9C5B8AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Guidance" sheetId="11" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1861" uniqueCount="1203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1863" uniqueCount="1203">
   <si>
     <t>Region</t>
   </si>
@@ -7650,8 +7650,8 @@
   </sheetPr>
   <dimension ref="A1:AD50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7805,11 +7805,11 @@
         <v>271588</v>
       </c>
       <c r="H2" s="41" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I2" s="1">
         <f>IF(ISNA(VLOOKUP(H2,'Base Locations'!A1:F341,2)),"",VLOOKUP(H2,'Base Locations'!A1:F341,2))</f>
-        <v>817181</v>
+        <v>450049</v>
       </c>
       <c r="J2" s="41" t="s">
         <v>52</v>
@@ -7817,7 +7817,9 @@
       <c r="K2" s="41" t="s">
         <v>409</v>
       </c>
-      <c r="L2" s="41"/>
+      <c r="L2" s="41" t="s">
+        <v>408</v>
+      </c>
       <c r="M2" s="41" t="s">
         <v>1169</v>
       </c>
@@ -7825,10 +7827,12 @@
         <f>IF(ISNA(VLOOKUP(M2,Services!$A$1:$B$45,2)),"",VLOOKUP(M2,Services!$A$1:$B$45,2))</f>
         <v>BHA3</v>
       </c>
-      <c r="O2" s="41"/>
+      <c r="O2" s="41" t="s">
+        <v>1168</v>
+      </c>
       <c r="P2" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(O2,Services!$A$1:$B$45,2)),"",VLOOKUP(O2,Services!$A$1:$B$45,2))</f>
-        <v/>
+        <v>BAB2</v>
       </c>
       <c r="Q2" s="41"/>
       <c r="R2" s="1" t="str">

</xml_diff>